<commit_message>
update email route from backend
</commit_message>
<xml_diff>
--- a/wording-parser/Lang-Locale.xlsx
+++ b/wording-parser/Lang-Locale.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
   <si>
     <t>Key</t>
   </si>
@@ -522,7 +522,7 @@
     <t xml:space="preserve">Enter the email address to search</t>
   </si>
   <si>
-    <t>email.username</t>
+    <t>email.email</t>
   </si>
   <si>
     <t>email.password</t>
@@ -561,6 +561,15 @@
     <t xml:space="preserve">Please input password</t>
   </si>
   <si>
+    <t>email.message.delete.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn có chắc chắn muốn xóa email?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to delete email?</t>
+  </si>
+  <si>
     <t>proxy.title</t>
   </si>
   <si>
@@ -679,6 +688,12 @@
   </si>
   <si>
     <t>Error</t>
+  </si>
+  <si>
+    <t>message.confirm</t>
+  </si>
+  <si>
+    <t>message.cancel</t>
   </si>
   <si>
     <t>permission.addRole</t>
@@ -932,7 +947,8 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
@@ -1479,7 +1495,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A56" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2144,10 +2160,10 @@
         <v>169</v>
       </c>
       <c r="B60" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>131</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61">
@@ -2206,25 +2222,25 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s">
+      <c r="A66" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B66" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" t="s">
-        <v>9</v>
+      <c r="B66" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B67" t="s">
-        <v>184</v>
+        <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>185</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68">
@@ -2320,95 +2336,95 @@
         <v>210</v>
       </c>
       <c r="B76" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="C76" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B77" t="s">
         <v>190</v>
       </c>
       <c r="C77" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C78" s="1" t="s">
+      <c r="A78" t="s">
         <v>215</v>
       </c>
+      <c r="B78" t="s">
+        <v>193</v>
+      </c>
+      <c r="C78" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="2" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="2" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="s">
+      <c r="A81" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="2" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="s">
+      <c r="A82" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B82" t="s">
-        <v>223</v>
-      </c>
-      <c r="C82" t="s">
-        <v>194</v>
+      <c r="B82" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="s">
+      <c r="A83" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B83" t="s">
-        <v>223</v>
-      </c>
-      <c r="C83" t="s">
-        <v>227</v>
+      <c r="B83" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B84" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C84" t="s">
         <v>229</v>
@@ -2419,21 +2435,21 @@
         <v>230</v>
       </c>
       <c r="B85" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C85" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
+        <v>231</v>
+      </c>
+      <c r="B86" t="s">
+        <v>228</v>
+      </c>
+      <c r="C86" t="s">
         <v>232</v>
-      </c>
-      <c r="B86" t="s">
-        <v>223</v>
-      </c>
-      <c r="C86" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="87">
@@ -2441,43 +2457,43 @@
         <v>233</v>
       </c>
       <c r="B87" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C87" t="s">
-        <v>203</v>
+        <v>234</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B88" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C88" t="s">
-        <v>200</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B89" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C89" t="s">
-        <v>236</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B90" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C90" t="s">
-        <v>238</v>
+        <v>206</v>
       </c>
     </row>
     <row r="91">
@@ -2485,153 +2501,153 @@
         <v>239</v>
       </c>
       <c r="B91" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C91" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
+        <v>240</v>
+      </c>
+      <c r="B92" t="s">
+        <v>228</v>
+      </c>
+      <c r="C92" t="s">
         <v>241</v>
-      </c>
-      <c r="B92" t="s">
-        <v>223</v>
-      </c>
-      <c r="C92" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
+        <v>242</v>
+      </c>
+      <c r="B93" t="s">
+        <v>228</v>
+      </c>
+      <c r="C93" t="s">
         <v>243</v>
-      </c>
-      <c r="B93" t="s">
-        <v>223</v>
-      </c>
-      <c r="C93" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
+        <v>244</v>
+      </c>
+      <c r="B94" t="s">
+        <v>228</v>
+      </c>
+      <c r="C94" t="s">
         <v>245</v>
-      </c>
-      <c r="B94" t="s">
-        <v>223</v>
-      </c>
-      <c r="C94" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
+        <v>246</v>
+      </c>
+      <c r="B95" t="s">
+        <v>228</v>
+      </c>
+      <c r="C95" t="s">
         <v>247</v>
-      </c>
-      <c r="B95" t="s">
-        <v>223</v>
-      </c>
-      <c r="C95" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
+        <v>248</v>
+      </c>
+      <c r="B96" t="s">
+        <v>228</v>
+      </c>
+      <c r="C96" t="s">
         <v>249</v>
-      </c>
-      <c r="B96" t="s">
-        <v>223</v>
-      </c>
-      <c r="C96" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
+        <v>250</v>
+      </c>
+      <c r="B97" t="s">
+        <v>228</v>
+      </c>
+      <c r="C97" t="s">
         <v>251</v>
-      </c>
-      <c r="B97" t="s">
-        <v>223</v>
-      </c>
-      <c r="C97" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
+        <v>252</v>
+      </c>
+      <c r="B98" t="s">
+        <v>228</v>
+      </c>
+      <c r="C98" t="s">
         <v>253</v>
-      </c>
-      <c r="B98" t="s">
-        <v>223</v>
-      </c>
-      <c r="C98" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
+        <v>254</v>
+      </c>
+      <c r="B99" t="s">
+        <v>228</v>
+      </c>
+      <c r="C99" t="s">
         <v>255</v>
-      </c>
-      <c r="B99" t="s">
-        <v>223</v>
-      </c>
-      <c r="C99" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
+        <v>256</v>
+      </c>
+      <c r="B100" t="s">
+        <v>228</v>
+      </c>
+      <c r="C100" t="s">
         <v>257</v>
-      </c>
-      <c r="B100" t="s">
-        <v>223</v>
-      </c>
-      <c r="C100" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
+        <v>258</v>
+      </c>
+      <c r="B101" t="s">
+        <v>228</v>
+      </c>
+      <c r="C101" t="s">
         <v>259</v>
-      </c>
-      <c r="B101" t="s">
-        <v>223</v>
-      </c>
-      <c r="C101" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
+        <v>260</v>
+      </c>
+      <c r="B102" t="s">
+        <v>228</v>
+      </c>
+      <c r="C102" t="s">
         <v>261</v>
-      </c>
-      <c r="B102" t="s">
-        <v>223</v>
-      </c>
-      <c r="C102" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
+        <v>262</v>
+      </c>
+      <c r="B103" t="s">
+        <v>228</v>
+      </c>
+      <c r="C103" t="s">
         <v>263</v>
-      </c>
-      <c r="B103" t="s">
-        <v>223</v>
-      </c>
-      <c r="C103" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
+        <v>264</v>
+      </c>
+      <c r="B104" t="s">
+        <v>228</v>
+      </c>
+      <c r="C104" t="s">
         <v>265</v>
-      </c>
-      <c r="B104" t="s">
-        <v>223</v>
-      </c>
-      <c r="C104" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="105">
@@ -2639,54 +2655,54 @@
         <v>266</v>
       </c>
       <c r="B105" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C105" t="s">
-        <v>188</v>
+        <v>267</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B106" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C106" t="s">
-        <v>209</v>
+        <v>269</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B107" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C107" t="s">
-        <v>269</v>
+        <v>209</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B108" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C108" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B109" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C109" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
     </row>
     <row r="110">
@@ -2694,7 +2710,7 @@
         <v>273</v>
       </c>
       <c r="B110" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C110" t="s">
         <v>274</v>
@@ -2705,32 +2721,32 @@
         <v>275</v>
       </c>
       <c r="B111" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C111" t="s">
-        <v>276</v>
+        <v>172</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
+        <v>276</v>
+      </c>
+      <c r="B112" t="s">
+        <v>228</v>
+      </c>
+      <c r="C112" t="s">
         <v>277</v>
-      </c>
-      <c r="B112" t="s">
-        <v>223</v>
-      </c>
-      <c r="C112" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
+        <v>278</v>
+      </c>
+      <c r="B113" t="s">
+        <v>228</v>
+      </c>
+      <c r="C113" t="s">
         <v>279</v>
-      </c>
-      <c r="B113" t="s">
-        <v>223</v>
-      </c>
-      <c r="C113" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="114">
@@ -2738,32 +2754,32 @@
         <v>280</v>
       </c>
       <c r="B114" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C114" t="s">
-        <v>194</v>
+        <v>281</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B115" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C115" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B116" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C116" t="s">
-        <v>284</v>
+        <v>175</v>
       </c>
     </row>
     <row r="117">
@@ -2771,7 +2787,7 @@
         <v>285</v>
       </c>
       <c r="B117" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C117" t="s">
         <v>197</v>
@@ -2782,54 +2798,54 @@
         <v>286</v>
       </c>
       <c r="B118" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C118" t="s">
-        <v>200</v>
+        <v>287</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B119" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C119" t="s">
-        <v>203</v>
+        <v>289</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B120" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C120" t="s">
-        <v>289</v>
+        <v>200</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B121" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C121" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B122" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C122" t="s">
-        <v>292</v>
+        <v>206</v>
       </c>
     </row>
     <row r="123">
@@ -2837,10 +2853,43 @@
         <v>293</v>
       </c>
       <c r="B123" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C123" t="s">
         <v>294</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>295</v>
+      </c>
+      <c r="B124" t="s">
+        <v>228</v>
+      </c>
+      <c r="C124" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>296</v>
+      </c>
+      <c r="B125" t="s">
+        <v>228</v>
+      </c>
+      <c r="C125" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>298</v>
+      </c>
+      <c r="B126" t="s">
+        <v>228</v>
+      </c>
+      <c r="C126" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add create template using tinymce
</commit_message>
<xml_diff>
--- a/wording-parser/Lang-Locale.xlsx
+++ b/wording-parser/Lang-Locale.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="207">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -77,6 +77,33 @@
   </si>
   <si>
     <t xml:space="preserve">Template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">route.templateList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danh sách bản mẫu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List Template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">route.createTemplate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tạo bản mẫu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">route.editTemplate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sửa bản mẫu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Template</t>
   </si>
   <si>
     <t xml:space="preserve">navbar.logOut</t>
@@ -715,15 +742,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C67" activeCellId="0" sqref="C67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33"/>
   </cols>
@@ -805,7 +832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>19</v>
       </c>
@@ -816,48 +843,48 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -997,175 +1024,175 @@
         <v>68</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C28" s="0" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,120 +1200,120 @@
         <v>105</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C44" s="0" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>119</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>121</v>
+        <v>48</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>122</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,142 +1332,142 @@
         <v>129</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>136</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>18</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>70</v>
+        <v>142</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>146</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>155</v>
+        <v>87</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>156</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1454,7 +1481,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>160</v>
       </c>
@@ -1465,7 +1492,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>163</v>
       </c>
@@ -1476,7 +1503,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>166</v>
       </c>
@@ -1547,54 +1574,54 @@
         <v>184</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,21 +1629,54 @@
         <v>196</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>174</v>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new route: schedule run
</commit_message>
<xml_diff>
--- a/wording-parser/Lang-Locale.xlsx
+++ b/wording-parser/Lang-Locale.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="211">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -106,6 +106,15 @@
     <t xml:space="preserve">Edit Template</t>
   </si>
   <si>
+    <t xml:space="preserve">route.scheduleRun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lịch trình chạy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schedule Run</t>
+  </si>
+  <si>
     <t xml:space="preserve">navbar.logOut</t>
   </si>
   <si>
@@ -527,6 +536,9 @@
   </si>
   <si>
     <t xml:space="preserve">Do you want to delete this template?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.title</t>
   </si>
   <si>
     <t xml:space="preserve">button.add</t>
@@ -742,13 +754,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34"/>
@@ -865,8 +877,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -881,21 +893,21 @@
         <v>31</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1057,21 +1069,21 @@
         <v>77</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C29" s="0" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,15 +1105,15 @@
         <v>85</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>88</v>
@@ -1129,26 +1141,26 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1156,32 +1168,32 @@
         <v>99</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1189,21 +1201,21 @@
         <v>104</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,26 +1245,26 @@
         <v>114</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C45" s="0" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>82</v>
@@ -1263,13 +1275,13 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1288,15 +1300,15 @@
         <v>123</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>48</v>
@@ -1307,24 +1319,24 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1365,54 +1377,54 @@
         <v>138</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="0" t="s">
         <v>143</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B60" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C60" s="0" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1420,15 +1432,15 @@
         <v>149</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>80</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>82</v>
@@ -1439,21 +1451,21 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>154</v>
+        <v>36</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>155</v>
@@ -1464,21 +1476,21 @@
         <v>156</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>87</v>
+        <v>157</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>88</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>158</v>
+        <v>90</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>159</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1514,7 +1526,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>169</v>
       </c>
@@ -1530,106 +1542,106 @@
         <v>172</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>173</v>
+        <v>29</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C72" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="B72" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C73" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="B73" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C74" s="0" t="s">
         <v>181</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C75" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="B75" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C76" s="0" t="s">
         <v>187</v>
-      </c>
-      <c r="B76" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C77" s="0" t="s">
         <v>190</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C78" s="0" t="s">
         <v>193</v>
-      </c>
-      <c r="B78" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B79" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="B79" s="0" t="s">
-        <v>173</v>
-      </c>
       <c r="C79" s="0" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>198</v>
@@ -1640,32 +1652,32 @@
         <v>199</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C82" s="0" t="s">
         <v>202</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C83" s="0" t="s">
         <v>205</v>
-      </c>
-      <c r="B83" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,10 +1685,32 @@
         <v>206</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>183</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update email with proxy
</commit_message>
<xml_diff>
--- a/wording-parser/Lang-Locale.xlsx
+++ b/wording-parser/Lang-Locale.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="225">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -364,6 +364,15 @@
     <t xml:space="preserve">Please input password</t>
   </si>
   <si>
+    <t xml:space="preserve">email.validate.proxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vui lòng chọn proxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please select proxy</t>
+  </si>
+  <si>
     <t xml:space="preserve">email.message.delete</t>
   </si>
   <si>
@@ -373,6 +382,48 @@
     <t xml:space="preserve">Do you want to delete email?</t>
   </si>
   <si>
+    <t xml:space="preserve">email.proxyId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email.proxyName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email.proxyHost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Máy chủ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email.proxyPort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cổng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email.proxyUsername</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email.proxyPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email.proxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email.proxyInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thông tin Proxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proxy Info</t>
+  </si>
+  <si>
     <t xml:space="preserve">proxy.title</t>
   </si>
   <si>
@@ -385,21 +436,9 @@
     <t xml:space="preserve">proxy.host</t>
   </si>
   <si>
-    <t xml:space="preserve">Máy chủ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Host</t>
-  </si>
-  <si>
     <t xml:space="preserve">proxy.port</t>
   </si>
   <si>
-    <t xml:space="preserve">Cổng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port</t>
-  </si>
-  <si>
     <t xml:space="preserve">proxy.username</t>
   </si>
   <si>
@@ -539,6 +578,9 @@
   </si>
   <si>
     <t xml:space="preserve">scheduleRun.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button.close</t>
   </si>
   <si>
     <t xml:space="preserve">button.add</t>
@@ -754,13 +796,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34"/>
@@ -1240,7 +1282,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>114</v>
       </c>
@@ -1256,15 +1298,15 @@
         <v>117</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>82</v>
@@ -1275,7 +1317,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>85</v>
@@ -1286,29 +1328,29 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>48</v>
@@ -1319,7 +1361,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>51</v>
@@ -1330,35 +1372,35 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>133</v>
+        <v>12</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>134</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1366,351 +1408,461 @@
         <v>135</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>136</v>
+        <v>82</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>137</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>140</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>151</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>36</v>
+        <v>149</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>164</v>
+        <v>158</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>167</v>
+        <v>17</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>168</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B74" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="C74" s="0" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="B71" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="B75" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B76" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C76" s="0" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B77" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C77" s="0" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B78" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="C74" s="0" t="s">
+      <c r="C78" s="0" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B79" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="C79" s="0" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B76" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="B78" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="B79" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>174</v>
+        <v>29</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>177</v>
+        <v>57</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>178</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C89" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="B86" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>187</v>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update show list schedule run cronjob
</commit_message>
<xml_diff>
--- a/wording-parser/Lang-Locale.xlsx
+++ b/wording-parser/Lang-Locale.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="240">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -578,6 +578,51 @@
   </si>
   <si>
     <t xml:space="preserve">scheduleRun.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhập email hoặc tên bản mẫu để tìm kiếm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input email or template name to search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.emailTos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gửi tới</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.proxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.schedule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trạng thái</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.actions</t>
   </si>
   <si>
     <t xml:space="preserve">button.close</t>
@@ -704,7 +749,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -726,6 +771,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -770,12 +821,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -796,13 +851,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B90" activeCellId="0" sqref="B90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34"/>
@@ -1694,175 +1749,274 @@
         <v>186</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>57</v>
+        <v>187</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>188</v>
+        <v>82</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>190</v>
       </c>
       <c r="B83" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="B84" s="0" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="C84" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="B84" s="0" t="s">
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="C84" s="0" t="s">
+      <c r="B85" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="B86" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="B87" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C85" s="0" t="s">
+      <c r="B88" s="0" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="C88" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="B86" s="0" t="s">
+    </row>
+    <row r="89" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C86" s="0" t="s">
+      <c r="B89" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="B87" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="B88" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B89" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
-        <v>211</v>
-      </c>
       <c r="B90" s="0" t="s">
-        <v>188</v>
+        <v>57</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>212</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B98" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="B96" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="C96" s="0" t="s">
-        <v>201</v>
+      <c r="C98" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update edit, change status cronjob schedule
</commit_message>
<xml_diff>
--- a/wording-parser/Lang-Locale.xlsx
+++ b/wording-parser/Lang-Locale.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="249">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -619,10 +619,37 @@
     <t xml:space="preserve">Trạng thái</t>
   </si>
   <si>
-    <t xml:space="preserve">Enable</t>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.status.false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tắt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.status.true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bật</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On</t>
   </si>
   <si>
     <t xml:space="preserve">scheduleRun.actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.message.modifyStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn có thật sự muốn thay đổi trạng thái?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to change status?</t>
   </si>
   <si>
     <t xml:space="preserve">button.close</t>
@@ -749,7 +776,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -771,12 +798,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -821,16 +842,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -851,13 +868,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B90" activeCellId="0" sqref="B90"/>
+      <selection pane="topLeft" activeCell="C92" activeCellId="0" sqref="C92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34"/>
@@ -1832,59 +1849,59 @@
         <v>199</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
         <v>200</v>
       </c>
       <c r="B89" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B91" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C89" s="0" t="s">
+      <c r="C91" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="B90" s="0" t="s">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B93" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="C93" s="0" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="B91" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="B92" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B93" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1947,54 +1964,54 @@
         <v>226</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2002,21 +2019,54 @@
         <v>238</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>219</v>
+        <v>240</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>216</v>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update reload data schedule
</commit_message>
<xml_diff>
--- a/wording-parser/Lang-Locale.xlsx
+++ b/wording-parser/Lang-Locale.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="255">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -316,6 +316,15 @@
     <t xml:space="preserve">Please select schedule cron</t>
   </si>
   <si>
+    <t xml:space="preserve">schedule.reload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Làm mới toàn bộ dữ liệu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reload all data</t>
+  </si>
+  <si>
     <t xml:space="preserve">email.title</t>
   </si>
   <si>
@@ -650,6 +659,15 @@
   </si>
   <si>
     <t xml:space="preserve">Do you want to change status?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduleRun.message.delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn có chắc chắn muốn xóa lịch trình chạy này?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to delete this schedule run?</t>
   </si>
   <si>
     <t xml:space="preserve">button.close</t>
@@ -868,10 +886,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C92" activeCellId="0" sqref="C92"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C95" activeCellId="0" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1266,26 +1284,26 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1293,32 +1311,32 @@
         <v>102</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1326,21 +1344,21 @@
         <v>107</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1354,7 +1372,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>114</v>
       </c>
@@ -1365,7 +1383,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>117</v>
       </c>
@@ -1376,37 +1394,37 @@
         <v>119</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>120</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1425,92 +1443,92 @@
         <v>128</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>49</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>134</v>
       </c>
       <c r="B54" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B55" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C55" s="0" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>126</v>
@@ -1521,46 +1539,46 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>49</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>143</v>
+        <v>90</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>144</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,54 +1619,54 @@
         <v>154</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>112</v>
+        <v>155</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>113</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>156</v>
+        <v>115</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="0" t="s">
         <v>159</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B70" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="0" t="s">
+      <c r="C70" s="0" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,40 +1674,40 @@
         <v>165</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>82</v>
+        <v>166</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>83</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>168</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>170</v>
+        <v>36</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>171</v>
@@ -1700,21 +1718,21 @@
         <v>172</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>90</v>
+        <v>173</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>91</v>
+        <v>174</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>174</v>
+        <v>90</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>175</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,26 +1768,26 @@
         <v>184</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>185</v>
       </c>
       <c r="B80" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B81" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C80" s="0" t="s">
+      <c r="C81" s="0" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="B81" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1777,32 +1795,32 @@
         <v>189</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>82</v>
+        <v>190</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>83</v>
+        <v>191</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>192</v>
+        <v>10</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>193</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,43 +1828,43 @@
         <v>194</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>12</v>
+        <v>195</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>12</v>
+        <v>196</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>198</v>
+        <v>17</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>199</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,7 +1879,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="0" t="s">
         <v>203</v>
       </c>
       <c r="B90" s="0" t="s">
@@ -1871,59 +1889,59 @@
         <v>205</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>206</v>
       </c>
       <c r="B91" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B92" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C91" s="0" t="s">
+      <c r="C92" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B92" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>209</v>
-      </c>
-    </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+      <c r="A93" s="1" t="s">
         <v>210</v>
       </c>
       <c r="B93" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B95" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C93" s="0" t="s">
+      <c r="C95" s="0" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="B94" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="B95" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="C95" s="0" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1997,43 +2015,43 @@
         <v>235</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,21 +2070,43 @@
         <v>247</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>227</v>
+        <v>248</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>224</v>
+        <v>251</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>225</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update email add sender name
</commit_message>
<xml_diff>
--- a/wording-parser/Lang-Locale.xlsx
+++ b/wording-parser/Lang-Locale.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="270">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -331,10 +331,47 @@
     <t xml:space="preserve">email.search</t>
   </si>
   <si>
-    <t xml:space="preserve">Nhập email để tìm kiếm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter the email address to search</t>
+    <t xml:space="preserve">Nhập email hoặc tên người gửi để tìm kiếm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Enter the email address or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">sender name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to search</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">email.emailName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên người gửi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sender name</t>
   </si>
   <si>
     <t xml:space="preserve">email.email</t>
@@ -382,6 +419,15 @@
     <t xml:space="preserve">Please select proxy</t>
   </si>
   <si>
+    <t xml:space="preserve">email.validate.emailName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vui lòng nhập tên người gửi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please input sender name</t>
+  </si>
+  <si>
     <t xml:space="preserve">email.message.delete</t>
   </si>
   <si>
@@ -592,10 +638,10 @@
     <t xml:space="preserve">scheduleRun.search</t>
   </si>
   <si>
-    <t xml:space="preserve">Nhập email hoặc tên bản mẫu để tìm kiếm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input email or template name to search</t>
+    <t xml:space="preserve">Nhập email hoặc tên người gửi hoặc tên bản mẫu hoặc tên lịch trình để tìm kiếm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input email or sender name or template or schedule name to search</t>
   </si>
   <si>
     <t xml:space="preserve">scheduleRun.id</t>
@@ -821,7 +867,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -843,6 +889,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -913,10 +965,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A115" activeCellId="0" sqref="A115"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C85" activeCellId="0" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1333,7 +1385,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>102</v>
       </c>
@@ -1344,37 +1396,37 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>105</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>109</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1382,21 +1434,21 @@
         <v>110</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1410,7 +1462,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>117</v>
       </c>
@@ -1421,7 +1473,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>120</v>
       </c>
@@ -1437,43 +1489,43 @@
         <v>123</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,48 +1533,48 @@
         <v>131</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>49</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>51</v>
+        <v>135</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>135</v>
+        <v>51</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>12</v>
@@ -1533,101 +1585,101 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>49</v>
+        <v>133</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>51</v>
+        <v>135</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>147</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>149</v>
+        <v>90</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>150</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1657,131 +1709,131 @@
         <v>157</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>118</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>164</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>17</v>
+        <v>165</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>18</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>85</v>
+        <v>172</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>171</v>
+        <v>83</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>173</v>
+        <v>85</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>174</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>181</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1806,118 +1858,118 @@
         <v>187</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>188</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>29</v>
+        <v>189</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>30</v>
+        <v>190</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>10</v>
+        <v>196</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>10</v>
+        <v>197</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>195</v>
+        <v>82</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>196</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>14</v>
+        <v>201</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>15</v>
+        <v>202</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>202</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>204</v>
+        <v>17</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>205</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="0" t="s">
         <v>206</v>
       </c>
       <c r="B91" s="0" t="s">
@@ -1927,70 +1979,70 @@
         <v>208</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="s">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
         <v>209</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>90</v>
+        <v>210</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>91</v>
+        <v>211</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>214</v>
+        <v>90</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>215</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+      <c r="A95" s="1" t="s">
         <v>216</v>
       </c>
       <c r="B95" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="B97" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C95" s="0" t="s">
+      <c r="C97" s="0" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="B96" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="C96" s="0" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="B97" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="C97" s="0" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2064,43 +2116,43 @@
         <v>241</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2119,46 +2171,46 @@
         <v>253</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>233</v>
+        <v>254</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>234</v>
+        <v>255</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>231</v>
+        <v>258</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>261</v>
       </c>
@@ -2169,7 +2221,29 @@
         <v>263</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
new feature: add, edit template attachments
</commit_message>
<xml_diff>
--- a/wording-parser/Lang-Locale.xlsx
+++ b/wording-parser/Lang-Locale.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="282">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -334,35 +334,7 @@
     <t xml:space="preserve">Nhập email hoặc tên người gửi để tìm kiếm</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Enter the email address or </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">sender name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> to search</t>
-    </r>
+    <t xml:space="preserve">Enter the email address or sender name to search</t>
   </si>
   <si>
     <t xml:space="preserve">email.emailName</t>
@@ -630,6 +602,42 @@
   </si>
   <si>
     <t xml:space="preserve">Do you want to delete this template?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template.attachment.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tệp đính kèm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attachments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template.attachment.no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template.attachment.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template.attachment.actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template.attachment.delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn có chắc chắn muốn xóa tệp đính kèm này?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to delete this attachment?</t>
   </si>
   <si>
     <t xml:space="preserve">scheduleRun.title</t>
@@ -867,7 +875,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -889,12 +897,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -965,10 +967,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C116"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C85" activeCellId="0" sqref="C85"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C88" activeCellId="0" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1880,279 +1882,279 @@
         <v>193</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>194</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>29</v>
+        <v>195</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>30</v>
+        <v>196</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>196</v>
+        <v>111</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>82</v>
+        <v>200</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>83</v>
+        <v>201</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>14</v>
+        <v>208</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>207</v>
+        <v>10</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>208</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="s">
-        <v>212</v>
+      <c r="A93" s="0" t="s">
+        <v>215</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>213</v>
+        <v>12</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="s">
-        <v>215</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>216</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="s">
-        <v>216</v>
+      <c r="A95" s="0" t="s">
+        <v>217</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>217</v>
+        <v>17</v>
       </c>
       <c r="C95" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
+      <c r="B96" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B96" s="0" t="s">
+      <c r="C96" s="0" t="s">
         <v>220</v>
-      </c>
-      <c r="C96" s="0" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B97" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="B97" s="0" t="s">
+      <c r="C97" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B102" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C97" s="0" t="s">
+      <c r="C102" s="0" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="B98" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="C98" s="0" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="B99" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="C99" s="0" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="B100" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="C100" s="0" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="B101" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="C101" s="0" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="B102" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="C102" s="0" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>224</v>
+        <v>245</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="C107" s="0" t="s">
         <v>249</v>
-      </c>
-      <c r="B107" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="C107" s="0" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,57 +2195,112 @@
         <v>259</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>